<commit_message>
weird issues have been fixed
</commit_message>
<xml_diff>
--- a/invoice_automation/generated_invoices/INV-FY2526-001.xlsx
+++ b/invoice_automation/generated_invoices/INV-FY2526-001.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="1" state="visible" r:id="rId1"/>
@@ -734,6 +734,95 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>4</col>
+      <colOff>422555</colOff>
+      <row>1</row>
+      <rowOff>79151</rowOff>
+    </from>
+    <to>
+      <col>5</col>
+      <colOff>715504</colOff>
+      <row>6</row>
+      <rowOff>143297</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="x_image_1"/>
+        <cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5631803" y="273023"/>
+          <a:ext cx="1084347" cy="1033504"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>3</col>
+      <colOff>246654</colOff>
+      <row>30</row>
+      <rowOff>36736</rowOff>
+    </from>
+    <to>
+      <col>5</col>
+      <colOff>652565</colOff>
+      <row>33</row>
+      <rowOff>44532</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Picture 1"/>
+        <cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm>
+          <a:off x="5379133" y="5578554"/>
+          <a:ext cx="1733639" cy="558829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1027,28 +1116,28 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="121" zoomScaleNormal="113" zoomScaleSheetLayoutView="36" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:C37"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="121" zoomScaleNormal="113" zoomScaleSheetLayoutView="36" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col width="16.140625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
-    <col width="15.42578125" customWidth="1" style="1" min="2" max="2"/>
-    <col width="41.85546875" customWidth="1" style="1" min="3" max="3"/>
-    <col width="7.140625" customWidth="1" style="1" min="4" max="4"/>
-    <col width="11.85546875" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
-    <col width="13.7109375" customWidth="1" style="1" min="6" max="6"/>
-    <col width="9.140625" customWidth="1" style="1" min="7" max="7"/>
-    <col width="12.85546875" bestFit="1" customWidth="1" style="1" min="8" max="8"/>
-    <col width="9.140625" customWidth="1" style="1" min="9" max="16384"/>
+    <col width="16.1796875" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="15.453125" customWidth="1" style="1" min="2" max="2"/>
+    <col width="41.81640625" customWidth="1" style="1" min="3" max="3"/>
+    <col width="7.1796875" customWidth="1" style="1" min="4" max="4"/>
+    <col width="11.81640625" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
+    <col width="13.7265625" customWidth="1" style="1" min="6" max="6"/>
+    <col width="9.1796875" customWidth="1" style="1" min="7" max="7"/>
+    <col width="12.81640625" bestFit="1" customWidth="1" style="1" min="8" max="8"/>
+    <col width="9.1796875" customWidth="1" style="1" min="9" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="n"/>
       <c r="B1" s="91" t="inlineStr">
         <is>
-          <t>License Number: 797747 | INV-FY2526-022 | Tax ID : 100425748900003</t>
+          <t>License Number: 797747 | INV-FY2526-001 | Tax ID : 100425748900003</t>
         </is>
       </c>
       <c r="C1" s="92" t="n"/>
@@ -1184,7 +1273,7 @@
       </c>
       <c r="C12" s="23" t="inlineStr">
         <is>
-          <t>ACME Corporation</t>
+          <t>Unilever Master - GCC</t>
         </is>
       </c>
       <c r="D12" s="3" t="n"/>
@@ -1195,7 +1284,7 @@
       </c>
       <c r="F12" s="35" t="inlineStr">
         <is>
-          <t>30/01/2026</t>
+          <t>04/02/2026</t>
         </is>
       </c>
       <c r="G12" s="3" t="n"/>
@@ -1209,7 +1298,7 @@
       </c>
       <c r="C13" s="42" t="inlineStr">
         <is>
-          <t>123 Main St</t>
+          <t>Dubai Business Park, Dubai, UAE</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
@@ -1218,9 +1307,10 @@
           <t>Due Date:</t>
         </is>
       </c>
-      <c r="F13" s="35">
-        <f>F12+30</f>
-        <v/>
+      <c r="F13" s="35" t="inlineStr">
+        <is>
+          <t>06/03/2026</t>
+        </is>
       </c>
       <c r="G13" s="3" t="n"/>
     </row>
@@ -1229,7 +1319,7 @@
       <c r="B14" s="22" t="n"/>
       <c r="C14" s="42" t="inlineStr">
         <is>
-          <t>Suite 400</t>
+          <t>Dubai Business Park, Dubai, UAE</t>
         </is>
       </c>
       <c r="D14" s="3" t="n"/>
@@ -1250,7 +1340,7 @@
       <c r="B15" s="22" t="n"/>
       <c r="C15" s="42" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Dubai Business Park, Dubai, UAE</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
@@ -1261,7 +1351,7 @@
       </c>
       <c r="F15" s="36" t="inlineStr">
         <is>
-          <t>BO-100</t>
+          <t>NAPP|2026|02</t>
         </is>
       </c>
       <c r="G15" s="3" t="n"/>
@@ -1275,7 +1365,7 @@
       </c>
       <c r="C16" s="24" t="inlineStr">
         <is>
-          <t>TRN-987654321</t>
+          <t>101010</t>
         </is>
       </c>
       <c r="D16" s="3" t="n"/>
@@ -1354,19 +1444,17 @@
       </c>
       <c r="C21" s="41" t="inlineStr">
         <is>
-          <t>APAC K-Celeb W2 Youku | Oct'2025</t>
+          <t>Napptix delivery</t>
         </is>
       </c>
       <c r="D21" s="39" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="E21" s="55" t="n">
         <v>10</v>
       </c>
-      <c r="E21" s="55" t="n">
-        <v>500</v>
-      </c>
-      <c r="F21" s="55" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
+      <c r="F21" s="55" t="n">
+        <v>10000</v>
       </c>
       <c r="G21" s="3" t="n"/>
     </row>
@@ -1407,14 +1495,12 @@
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="F25" s="56" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
+      <c r="F25" s="56" t="n">
+        <v>10000</v>
       </c>
       <c r="G25" s="3" t="n"/>
     </row>
-    <row r="26" ht="22.5" customHeight="1">
+    <row r="26">
       <c r="A26" s="3" t="n"/>
       <c r="B26" s="2" t="inlineStr">
         <is>
@@ -1423,15 +1509,17 @@
       </c>
       <c r="C26" s="57" t="inlineStr">
         <is>
-          <t>Dollars Four Thousand Thirty Four and Cents Seventy Nine Only</t>
+          <t>TEN THOUSAND FIVE HUNDRED DOLLARS</t>
         </is>
       </c>
       <c r="D26" s="9" t="n"/>
-      <c r="E26" s="46" t="n">
-        <v>5</v>
+      <c r="E26" s="46" t="inlineStr">
+        <is>
+          <t>VAT(5%)</t>
+        </is>
       </c>
       <c r="F26" s="56" t="n">
-        <v>0.025</v>
+        <v>500</v>
       </c>
       <c r="G26" s="3" t="n"/>
     </row>
@@ -1719,5 +1807,6 @@
   </hyperlinks>
   <pageMargins left="0.7086614173228346" right="0" top="1.181102362204724" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="portrait" paperSize="9"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>